<commit_message>
Borrado de ejemplos en el cuadro de incidencias
Cuadro de incidencias vacio para poder registrar desde el inicio
</commit_message>
<xml_diff>
--- a/Incidencias/Incidencias.xlsx
+++ b/Incidencias/Incidencias.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Incidencia</t>
   </si>
@@ -66,9 +66,6 @@
     <t>BAJA</t>
   </si>
   <si>
-    <t>EL LOGIN NO FUNCIONA</t>
-  </si>
-  <si>
     <t>PENDIENTE</t>
   </si>
   <si>
@@ -79,25 +76,13 @@
   </si>
   <si>
     <t>codigo</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>Funciona mierda no me jodan!</t>
-  </si>
-  <si>
-    <t>yo</t>
-  </si>
-  <si>
-    <t>may</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -248,9 +233,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,13 +247,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,21 +528,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="80" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
@@ -569,55 +551,55 @@
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75">
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -625,7 +607,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -633,12 +615,12 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="18" t="s">
-        <v>19</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -659,70 +641,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="24.95" customHeight="1">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6">
-        <v>41891</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1">
-      <c r="A10" s="4">
-        <v>2</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6">
-        <v>41891</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1">
-      <c r="A11" s="4">
-        <v>3</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="21">
-        <v>41891</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1">
+    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -731,7 +677,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="24.95" customHeight="1">
+    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -740,7 +686,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1">
+    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -749,7 +695,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" ht="24.95" customHeight="1">
+    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -758,7 +704,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="24.95" customHeight="1">
+    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -767,7 +713,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="24.95" customHeight="1">
+    <row r="17" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -776,7 +722,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="24.95" customHeight="1">
+    <row r="18" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -785,7 +731,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" ht="24.95" customHeight="1">
+    <row r="19" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -794,7 +740,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="24.95" customHeight="1">
+    <row r="20" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -803,7 +749,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" ht="24.95" customHeight="1">
+    <row r="21" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -812,7 +758,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="24.95" customHeight="1">
+    <row r="22" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -821,7 +767,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="24.95" customHeight="1">
+    <row r="23" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -830,7 +776,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="24.95" customHeight="1">
+    <row r="24" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -839,7 +785,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="24.95" customHeight="1">
+    <row r="25" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -848,7 +794,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="24.95" customHeight="1">
+    <row r="26" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -857,7 +803,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="24.95" customHeight="1">
+    <row r="27" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -866,7 +812,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="24.95" customHeight="1">
+    <row r="28" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -875,7 +821,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="24.95" customHeight="1">
+    <row r="29" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -884,7 +830,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="24.95" customHeight="1">
+    <row r="30" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -893,7 +839,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="24.95" customHeight="1">
+    <row r="31" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -902,7 +848,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -911,7 +857,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -920,7 +866,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -929,7 +875,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -938,7 +884,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -947,7 +893,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -956,7 +902,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -965,7 +911,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -974,8 +920,8 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7">
-      <c r="B40" s="17"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="16"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>

</xml_diff>

<commit_message>
Agregar mensaje de Bienvenida
Falta mensaje de bienvenida al sistema
</commit_message>
<xml_diff>
--- a/Incidencias/Incidencias.xlsx
+++ b/Incidencias/Incidencias.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Incidencia</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Al momento de actualizar un tutor no aparece ninguna ventana de " registro actualizado con éxito"</t>
+  </si>
+  <si>
+    <t>Falta mensaje de "Bienvenido" al ingresar al sistema</t>
   </si>
 </sst>
 </file>
@@ -257,10 +260,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -535,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,7 +549,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,10 +568,10 @@
       <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -685,7 +688,7 @@
       <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="18"/>
@@ -706,19 +709,31 @@
       <c r="E11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="A12" s="4">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="6">
+        <v>41931</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>

</xml_diff>